<commit_message>
Add blood-type enum and regen
</commit_message>
<xml_diff>
--- a/docs/donor/donor.xlsx
+++ b/docs/donor/donor.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
+    <sheet name="blood_type list" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -168,12 +169,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>age_value</t>
   </si>
   <si>
     <t>blood_type</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
   <si>
     <t>body_mass_index_value</t>
@@ -566,38 +579,41 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="A2:A1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: A / B / AB / O." sqref="B2:B1048576">
+      <formula1>'blood_type list'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="C2:C1048576">
       <formula1>-1e+307</formula1>
@@ -615,4 +631,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add "none of the above"
</commit_message>
<xml_diff>
--- a/docs/donor/donor.xlsx
+++ b/docs/donor/donor.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>age_value</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>None of the above</t>
   </si>
   <si>
     <t>body_mass_index_value</t>
@@ -579,31 +582,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -612,8 +615,8 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: A / B / AB / O." sqref="B2:B1048576">
-      <formula1>'blood_type list'!$A$1:$A$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: A / B / AB / O / None of the above." sqref="B2:B1048576">
+      <formula1>'blood_type list'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="C2:C1048576">
       <formula1>-1e+307</formula1>
@@ -635,7 +638,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -661,6 +664,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update docs after change of donor-v0.yaml
</commit_message>
<xml_diff>
--- a/docs/donor/donor.xlsx
+++ b/docs/donor/donor.xlsx
@@ -68,7 +68,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Desired value for blood_type</t>
+          <t>An individual's weight in kilograms divided by the square of the height in meters.</t>
         </r>
       </text>
     </comment>
@@ -81,7 +81,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>An individual's weight in kilograms divided by the square of the height in meters.</t>
+          <t>The circumstance or condition that caused death.</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The circumstance or condition that caused death.</t>
+          <t>Unit for height measurement.</t>
         </r>
       </text>
     </comment>
@@ -107,24 +107,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Unit for height measurement.</t>
+          <t>The vertical measurement or distance from the base to the top of a subject or participant.</t>
         </r>
       </text>
     </comment>
     <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The vertical measurement or distance from the base to the top of a subject or participant.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -138,6 +125,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mechanism of injury may be, for example: fall, impact (eg: auto accident), weapon (eg: firearm), etc.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J1" authorId="0">
       <text>
         <r>
@@ -147,7 +147,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Mechanism of injury may be, for example: fall, impact (eg: auto accident), weapon (eg: firearm), etc.</t>
+          <t>A record of a patient's background regarding health and the occurrence of disease events of the individual.</t>
         </r>
       </text>
     </comment>
@@ -160,7 +160,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A record of a patient's background regarding health and the occurrence of disease events of the individual.</t>
+          <t>A grouping of humans based on shared physical characteristics or social/ethnic identity generally viewed as distinct.</t>
         </r>
       </text>
     </comment>
@@ -173,7 +173,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A grouping of humans based on shared physical characteristics or social/ethnic identity generally viewed as distinct.</t>
+          <t>Biological sex at birth: male or female or other.</t>
         </r>
       </text>
     </comment>
@@ -186,24 +186,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Biological sex at birth: male or female or other.</t>
+          <t>Unit for weight measurement.</t>
         </r>
       </text>
     </comment>
     <comment ref="N1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Unit for weight measurement.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>age_unit</t>
   </si>
@@ -242,12 +229,6 @@
   </si>
   <si>
     <t>O</t>
-  </si>
-  <si>
-    <t>Submitter Suggestion</t>
-  </si>
-  <si>
-    <t>blood_type_suggested</t>
   </si>
   <si>
     <t>body_mass_index_value</t>
@@ -629,7 +610,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -638,7 +619,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,40 +630,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -691,10 +669,14 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: A / B / AB / O / Submitter Suggestion." sqref="C2:C1048576">
-      <formula1>'blood_type list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: A / B / AB / O." sqref="C2:C1048576">
+      <formula1>'blood_type list'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="E2:E1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="D2:D1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="G2:G1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -702,11 +684,7 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="I2:I1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="O2:O1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="N2:N1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -718,7 +696,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -744,11 +722,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>